<commit_message>
modifies e2e upload test encoding type
</commit_message>
<xml_diff>
--- a/conference-app/tests/e2e/data/smaller-2.xlsx
+++ b/conference-app/tests/e2e/data/smaller-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -49,58 +49,62 @@
     <t xml:space="preserve">Day</t>
   </si>
   <si>
+    <t xml:space="preserve">Welcome and introduction, including Welcome to Country by Barry McGuire Speaker
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plenary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Ballroom 2 &amp; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a Carneiro, AB Fourie, The University of Western Australia, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a Carneiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEYNOTE: Why should we ‘Think Big’ on closure? L Tyler, J Heyes, BHP, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura Tyler, BHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laura Tyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rehabilitation of the North End Box Cut (NEBC) dump at Tom Price mine operation: a legacy management case study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T Worthington, R Green, C Latham, B Yaqub, Rio Tinto Iron Ore, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T Worthington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problematic pit: closure liability to operational opportunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL Latham, C Lazo-Skold, Rio Tinto, Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL Latham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibition Area</t>
+  </si>
+  <si>
     <t xml:space="preserve">Welcome and introduction, including Welcome to Country by Barry McGuire Speaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plenary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Ballroom 2 &amp; 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a Carneiro, AB Fourie, The University of Western Australia, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a Carneiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEYNOTE: Why should we ‘Think Big’ on closure? L Tyler, J Heyes, BHP, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laura Tyler, BHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laura Tyler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rehabilitation of the North End Box Cut (NEBC) dump at Tom Price mine operation: a legacy management case study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T Worthington, R Green, C Latham, B Yaqub, Rio Tinto Iron Ore, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T Worthington</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problematic pit: closure liability to operational opportunity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL Latham, C Lazo-Skold, Rio Tinto, Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL Latham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morning Tea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Break</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exhibition Area</t>
   </si>
   <si>
     <t xml:space="preserve">AB Fourie</t>
@@ -117,7 +121,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m\/d\/yyyy\ h\:mm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -159,12 +163,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,6 +217,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,10 +229,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -254,10 +252,13 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="133.85"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -289,19 +290,19 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
+      <c r="C2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>43711.3333333333</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>43711.3541666667</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -313,7 +314,7 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -324,13 +325,13 @@
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="n">
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>43711.3541666667</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>43711.375</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -342,7 +343,7 @@
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -353,13 +354,13 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>43713.4375</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>43713.3958333333</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -371,7 +372,7 @@
       <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -382,13 +383,13 @@
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>43713.3958333333</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>43713.4166666667</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -400,7 +401,7 @@
       <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -411,38 +412,38 @@
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>43713.4166666667</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>43713.4375</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="2" t="n">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>43711.3333333333</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>43711.3541666667</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -451,10 +452,10 @@
       <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="2" t="n">
+      <c r="H7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -465,13 +466,13 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>43711.3541666667</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>43711.375</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -483,7 +484,7 @@
       <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -494,13 +495,13 @@
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="n">
+      <c r="C9" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <v>43713.375</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>43713.3958333333</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -512,7 +513,7 @@
       <c r="H9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -523,13 +524,13 @@
       <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3" t="n">
+      <c r="C10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="n">
         <v>43713.3958333333</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>43713.4166666667</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -539,9 +540,9 @@
         <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -552,25 +553,28 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>43713.4166666667</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>43713.4375</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="2" t="n">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="3" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="Welcome and introduction, including Welcome to Country by Barry McGuire Speaker&#10;"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>